<commit_message>
changed comma separators to periods & some re-wording
</commit_message>
<xml_diff>
--- a/Task1_KFC_Team/KFC-team_pizza-variables.xlsx
+++ b/Task1_KFC_Team/KFC-team_pizza-variables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/sule_kata_student_ceu_edu/Documents/DA-1_KFC-team_Team-Assignment-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\Data_ExercisesANDhomework_DA1\Task1_KFC_Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_9248653540E74473E8634A399E3E8C1851038385" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B982E8A-5D85-4296-AD8D-63DFCCC1B004}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C087B3-5F49-492D-94D7-2259DC74EE84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="1836" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -84,9 +84,6 @@
     <t>cust_rating</t>
   </si>
   <si>
-    <t>Qualitative variable. Google rating of the restaurant if the number of customer reviews exceed 50. Possible values are between 0 and 5.</t>
-  </si>
-  <si>
     <t>dist_CEU</t>
   </si>
   <si>
@@ -103,13 +100,16 @@
   </si>
   <si>
     <t>Qualitative variable. Name of delivery site where the delivery prices were collected from. Possible values are: NA (the price is for an on-site restaurant), Netpincér, Wolt.</t>
+  </si>
+  <si>
+    <t>Qualitative variable. Google rating of the restaurant if the number of customer reviews exceed 50. Possible values are between 1.0 and 5.0.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,16 +483,16 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="231" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -508,7 +508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -516,7 +516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -532,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -540,7 +540,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -548,7 +548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -556,36 +556,36 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>